<commit_message>
Updated group contribution file.
</commit_message>
<xml_diff>
--- a/Contibutions.xlsx
+++ b/Contibutions.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\napier-mail.napier.ac.uk\students\school of computing\user data\40346443\My Profile\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stanl\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E66FA1FE-9B23-4F45-8E93-BE86DCCEEF5C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13512"/>
+    <workbookView xWindow="7815" yWindow="1245" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Code Review 1</t>
   </si>
@@ -48,12 +55,15 @@
   </si>
   <si>
     <t>Oliwier: 40344894</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -364,23 +374,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -393,8 +403,11 @@
       <c r="E1" t="s">
         <v>7</v>
       </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -410,20 +423,48 @@
       <c r="E2">
         <v>25</v>
       </c>
+      <c r="F2">
+        <f>SUM(B2:E2)</f>
+        <v>100</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>26</v>
+      </c>
+      <c r="E3">
+        <v>26</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F5" si="0">SUM(B3:E3)</f>
+        <v>100</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>